<commit_message>
handle result object in scrapper.js
</commit_message>
<xml_diff>
--- a/event-tracker/reports/report_2023-09-26.xlsx
+++ b/event-tracker/reports/report_2023-09-26.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -414,12 +414,17 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>https://www.imdb.com/title/tt13622776/?ref_=hm_top_tt_i_1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
         <v>https://www.imdb.com/title/tt11737520/?ref_=hm_top_tt_i_2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resolve issue of no new data found
</commit_message>
<xml_diff>
--- a/event-tracker/reports/report_2023-09-26.xlsx
+++ b/event-tracker/reports/report_2023-09-26.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,19 +412,9 @@
         <v>https://www.imdb.com/title/tt13622776/?ref_=hm_top_tt_i_1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>https://www.imdb.com/title/tt13622776/?ref_=hm_top_tt_i_1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>https://www.imdb.com/title/tt11737520/?ref_=hm_top_tt_i_2</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>